<commit_message>
Added copyright to References
</commit_message>
<xml_diff>
--- a/References.xlsx
+++ b/References.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -130,6 +130,27 @@
   </si>
   <si>
     <t>http://developer.android.com/reference/android/widget/ListView.html#attr_android%3afooterDividersEnabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***********************************************************************************
+ Copyright © 2013 Deepika Punyamurtula
+ MyMoneyMate - Is an Open Source Android application to keep a record of your expenses.
+ This program is free software: you can redistribute it and/or modify it under 
+ the terms of the GNU General Public License as published by the Free Software Foundation, 
+ either version 3 of the License, or (at your option) any later version.
+ This program is distributed in the hope that it will be useful, but WITHOUT ANY WARRANTY; 
+ without even the implied warranty of MERCHANTABILITY or FITNESS FOR A PARTICULAR PURPOSE. 
+ See the GNU General Public License for more details.
+ You should have received a copy of the GNU General Public License along with this program.
+ If not, see http://www.gnu.org/licenses/
+ Please see the file "License" in this distribution for license terms. 
+ Below is the link to the License file:
+ https://github.com/udeepika/MyMoneyMate/blob/master/License.txt
+ Author - Deepika Punyamurtula
+ email:  udeepika@pdx.edu
+ Link to repository- https://github.com/udeepika/MyMoneyMate
+*******************************************************************************************
+</t>
   </si>
 </sst>
 </file>
@@ -182,10 +203,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -488,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,255 +524,263 @@
     <col min="3" max="3" width="108.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>7</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>8</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-    </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>9</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="1"/>
-    </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>10</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
-    </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>11</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>12</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:XFD1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C11" r:id="rId3"/>
-    <hyperlink ref="C26" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
-    <hyperlink ref="C24" r:id="rId6"/>
-    <hyperlink ref="C15" r:id="rId7"/>
-    <hyperlink ref="C19" r:id="rId8"/>
-    <hyperlink ref="C20" r:id="rId9"/>
-    <hyperlink ref="C10" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="C2" r:id="rId14"/>
-    <hyperlink ref="C4" r:id="rId15"/>
-    <hyperlink ref="C29" r:id="rId16"/>
-    <hyperlink ref="C31" r:id="rId17"/>
+    <hyperlink ref="C10" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C27" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C25" r:id="rId6"/>
+    <hyperlink ref="C16" r:id="rId7"/>
+    <hyperlink ref="C20" r:id="rId8"/>
+    <hyperlink ref="C21" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C7" r:id="rId13"/>
+    <hyperlink ref="C3" r:id="rId14"/>
+    <hyperlink ref="C5" r:id="rId15"/>
+    <hyperlink ref="C30" r:id="rId16"/>
+    <hyperlink ref="C32" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>

</xml_diff>